<commit_message>
fixes to the project matrix spreadsheet
</commit_message>
<xml_diff>
--- a/gudmap/projects/gudmap4/GUDMAP-Project-Matrix.xlsx
+++ b/gudmap/projects/gudmap4/GUDMAP-Project-Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristinawilliams/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535C30DD-1638-3A42-8B96-0798A3EDB023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAB68A8-E3DD-9546-BA51-ED92E001A79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27800" windowHeight="14580" xr2:uid="{A62D965B-578C-3541-A8BB-AFD7334F7B86}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="72">
   <si>
     <t>Chen/Ding</t>
   </si>
@@ -156,9 +156,6 @@
   </si>
   <si>
     <t>Bladder/Cloaca/UBlJ</t>
-  </si>
-  <si>
-    <t>Embryonic</t>
   </si>
   <si>
     <t>Juvenile</t>
@@ -794,47 +791,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -842,12 +857,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -883,18 +892,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1230,13 +1227,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C20BFEF4-4776-5C4D-968E-6ECFC6966944}">
-  <dimension ref="A1:Z91"/>
+  <dimension ref="A1:Z89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="W4" sqref="W4:X4"/>
+      <selection pane="bottomRight" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1267,7 +1264,7 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G2" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H2" s="21" t="s">
         <v>0</v>
@@ -1296,22 +1293,22 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
-      <c r="W2" s="99"/>
-      <c r="X2" s="99"/>
+      <c r="W2" s="103"/>
+      <c r="X2" s="103"/>
       <c r="Y2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="103"/>
       <c r="W3" s="111"/>
       <c r="X3" s="111"/>
     </row>
     <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="68" t="s">
         <v>68</v>
-      </c>
-      <c r="B4" s="68" t="s">
-        <v>69</v>
       </c>
       <c r="C4" s="66" t="s">
         <v>6</v>
@@ -1326,8 +1323,8 @@
       <c r="G4" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="103"/>
       <c r="W4" s="112"/>
       <c r="X4" s="112"/>
     </row>
@@ -1337,35 +1334,35 @@
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="103" t="s">
+      <c r="G5" s="107" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="107" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="104"/>
-      <c r="I5" s="104"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="105"/>
-      <c r="L5" s="103" t="s">
+      <c r="M5" s="109"/>
+      <c r="N5" s="107" t="s">
         <v>59</v>
       </c>
-      <c r="M5" s="105"/>
-      <c r="N5" s="103" t="s">
+      <c r="O5" s="109"/>
+      <c r="P5" s="107" t="s">
         <v>60</v>
       </c>
-      <c r="O5" s="105"/>
-      <c r="P5" s="103" t="s">
+      <c r="Q5" s="109"/>
+      <c r="R5" s="107" t="s">
         <v>61</v>
       </c>
-      <c r="Q5" s="105"/>
-      <c r="R5" s="103" t="s">
-        <v>62</v>
-      </c>
-      <c r="S5" s="106"/>
-      <c r="T5" s="104"/>
-      <c r="U5" s="104"/>
-      <c r="V5" s="104"/>
-      <c r="W5" s="104"/>
-      <c r="X5" s="104"/>
-      <c r="Y5" s="105"/>
+      <c r="S5" s="110"/>
+      <c r="T5" s="108"/>
+      <c r="U5" s="108"/>
+      <c r="V5" s="108"/>
+      <c r="W5" s="108"/>
+      <c r="X5" s="108"/>
+      <c r="Y5" s="109"/>
       <c r="Z5" s="74"/>
     </row>
     <row r="6" spans="1:26" s="15" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
@@ -1384,7 +1381,7 @@
         <v>17</v>
       </c>
       <c r="I6" s="85" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J6" s="86"/>
       <c r="K6" s="71" t="s">
@@ -1397,10 +1394,10 @@
         <v>19</v>
       </c>
       <c r="N6" s="69" t="s">
+        <v>70</v>
+      </c>
+      <c r="O6" s="71" t="s">
         <v>71</v>
-      </c>
-      <c r="O6" s="71" t="s">
-        <v>72</v>
       </c>
       <c r="P6" s="72" t="s">
         <v>13</v>
@@ -1408,19 +1405,19 @@
       <c r="Q6" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="R6" s="97" t="s">
+      <c r="R6" s="101" t="s">
+        <v>62</v>
+      </c>
+      <c r="S6" s="102"/>
+      <c r="T6" s="70" t="s">
         <v>63</v>
-      </c>
-      <c r="S6" s="98"/>
-      <c r="T6" s="70" t="s">
-        <v>64</v>
       </c>
       <c r="U6" s="85" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="86"/>
       <c r="W6" s="85" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="X6" s="86"/>
       <c r="Y6" s="71" t="s">
@@ -1455,8 +1452,8 @@
       <c r="O7" s="43"/>
       <c r="P7" s="30"/>
       <c r="Q7" s="29"/>
-      <c r="R7" s="93"/>
-      <c r="S7" s="78"/>
+      <c r="R7" s="95"/>
+      <c r="S7" s="92"/>
       <c r="T7" s="43"/>
       <c r="U7" s="75"/>
       <c r="V7" s="76"/>
@@ -1611,8 +1608,8 @@
       <c r="O12" s="43"/>
       <c r="P12" s="29"/>
       <c r="Q12" s="29"/>
-      <c r="R12" s="77"/>
-      <c r="S12" s="78"/>
+      <c r="R12" s="91"/>
+      <c r="S12" s="92"/>
       <c r="T12" s="43"/>
       <c r="U12" s="75"/>
       <c r="V12" s="76"/>
@@ -1624,7 +1621,7 @@
     <row r="13" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>31</v>
@@ -1646,8 +1643,8 @@
       <c r="O13" s="43"/>
       <c r="P13" s="30"/>
       <c r="Q13" s="29"/>
-      <c r="R13" s="93"/>
-      <c r="S13" s="78"/>
+      <c r="R13" s="95"/>
+      <c r="S13" s="92"/>
       <c r="T13" s="43"/>
       <c r="U13" s="75"/>
       <c r="V13" s="76"/>
@@ -1679,8 +1676,8 @@
       <c r="O14" s="43"/>
       <c r="P14" s="30"/>
       <c r="Q14" s="29"/>
-      <c r="R14" s="93"/>
-      <c r="S14" s="78"/>
+      <c r="R14" s="95"/>
+      <c r="S14" s="92"/>
       <c r="T14" s="43"/>
       <c r="U14" s="75"/>
       <c r="V14" s="76"/>
@@ -1712,8 +1709,8 @@
       <c r="O15" s="43"/>
       <c r="P15" s="30"/>
       <c r="Q15" s="29"/>
-      <c r="R15" s="93"/>
-      <c r="S15" s="78"/>
+      <c r="R15" s="95"/>
+      <c r="S15" s="92"/>
       <c r="T15" s="43"/>
       <c r="U15" s="75"/>
       <c r="V15" s="76"/>
@@ -1735,8 +1732,8 @@
       <c r="O16" s="43"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
-      <c r="R16" s="77"/>
-      <c r="S16" s="78"/>
+      <c r="R16" s="91"/>
+      <c r="S16" s="92"/>
       <c r="T16" s="43"/>
       <c r="U16" s="75"/>
       <c r="V16" s="76"/>
@@ -1770,8 +1767,8 @@
       <c r="O17" s="43"/>
       <c r="P17" s="30"/>
       <c r="Q17" s="29"/>
-      <c r="R17" s="93"/>
-      <c r="S17" s="78"/>
+      <c r="R17" s="95"/>
+      <c r="S17" s="92"/>
       <c r="T17" s="43"/>
       <c r="U17" s="75"/>
       <c r="V17" s="76"/>
@@ -1803,8 +1800,8 @@
       <c r="O18" s="43"/>
       <c r="P18" s="30"/>
       <c r="Q18" s="29"/>
-      <c r="R18" s="93"/>
-      <c r="S18" s="78"/>
+      <c r="R18" s="95"/>
+      <c r="S18" s="92"/>
       <c r="T18" s="43"/>
       <c r="U18" s="75"/>
       <c r="V18" s="76"/>
@@ -1836,8 +1833,8 @@
       <c r="O19" s="43"/>
       <c r="P19" s="30"/>
       <c r="Q19" s="29"/>
-      <c r="R19" s="93"/>
-      <c r="S19" s="78"/>
+      <c r="R19" s="95"/>
+      <c r="S19" s="92"/>
       <c r="T19" s="43"/>
       <c r="U19" s="75"/>
       <c r="V19" s="76"/>
@@ -1858,8 +1855,8 @@
       <c r="O20" s="43"/>
       <c r="P20" s="29"/>
       <c r="Q20" s="29"/>
-      <c r="R20" s="77"/>
-      <c r="S20" s="78"/>
+      <c r="R20" s="91"/>
+      <c r="S20" s="92"/>
       <c r="T20" s="43"/>
       <c r="U20" s="75"/>
       <c r="V20" s="76"/>
@@ -1883,8 +1880,8 @@
       <c r="O21" s="43"/>
       <c r="P21" s="29"/>
       <c r="Q21" s="29"/>
-      <c r="R21" s="77"/>
-      <c r="S21" s="78"/>
+      <c r="R21" s="91"/>
+      <c r="S21" s="92"/>
       <c r="T21" s="43"/>
       <c r="U21" s="75"/>
       <c r="V21" s="76"/>
@@ -1918,8 +1915,8 @@
       <c r="O22" s="43"/>
       <c r="P22" s="29"/>
       <c r="Q22" s="29"/>
-      <c r="R22" s="77"/>
-      <c r="S22" s="78"/>
+      <c r="R22" s="91"/>
+      <c r="S22" s="92"/>
       <c r="T22" s="43"/>
       <c r="U22" s="90"/>
       <c r="V22" s="76"/>
@@ -1951,8 +1948,8 @@
       <c r="O23" s="43"/>
       <c r="P23" s="29"/>
       <c r="Q23" s="29"/>
-      <c r="R23" s="77"/>
-      <c r="S23" s="78"/>
+      <c r="R23" s="91"/>
+      <c r="S23" s="92"/>
       <c r="T23" s="43"/>
       <c r="U23" s="90"/>
       <c r="V23" s="76"/>
@@ -1984,8 +1981,8 @@
       <c r="O24" s="43"/>
       <c r="P24" s="29"/>
       <c r="Q24" s="29"/>
-      <c r="R24" s="77"/>
-      <c r="S24" s="78"/>
+      <c r="R24" s="91"/>
+      <c r="S24" s="92"/>
       <c r="T24" s="42"/>
       <c r="U24" s="90"/>
       <c r="V24" s="76"/>
@@ -2017,8 +2014,8 @@
       <c r="O25" s="43"/>
       <c r="P25" s="29"/>
       <c r="Q25" s="29"/>
-      <c r="R25" s="77"/>
-      <c r="S25" s="78"/>
+      <c r="R25" s="91"/>
+      <c r="S25" s="92"/>
       <c r="T25" s="43"/>
       <c r="U25" s="90"/>
       <c r="V25" s="76"/>
@@ -2050,8 +2047,8 @@
       <c r="O26" s="43"/>
       <c r="P26" s="29"/>
       <c r="Q26" s="29"/>
-      <c r="R26" s="77"/>
-      <c r="S26" s="78"/>
+      <c r="R26" s="91"/>
+      <c r="S26" s="92"/>
       <c r="T26" s="43"/>
       <c r="U26" s="90"/>
       <c r="V26" s="76"/>
@@ -2083,8 +2080,8 @@
       <c r="O27" s="43"/>
       <c r="P27" s="30"/>
       <c r="Q27" s="29"/>
-      <c r="R27" s="93"/>
-      <c r="S27" s="78"/>
+      <c r="R27" s="95"/>
+      <c r="S27" s="92"/>
       <c r="T27" s="43"/>
       <c r="U27" s="75"/>
       <c r="V27" s="76"/>
@@ -2116,8 +2113,8 @@
       <c r="O28" s="43"/>
       <c r="P28" s="29"/>
       <c r="Q28" s="29"/>
-      <c r="R28" s="77"/>
-      <c r="S28" s="78"/>
+      <c r="R28" s="91"/>
+      <c r="S28" s="92"/>
       <c r="T28" s="43"/>
       <c r="U28" s="90"/>
       <c r="V28" s="76"/>
@@ -2149,8 +2146,8 @@
       <c r="O29" s="43"/>
       <c r="P29" s="30"/>
       <c r="Q29" s="29"/>
-      <c r="R29" s="93"/>
-      <c r="S29" s="78"/>
+      <c r="R29" s="95"/>
+      <c r="S29" s="92"/>
       <c r="T29" s="43"/>
       <c r="U29" s="75"/>
       <c r="V29" s="76"/>
@@ -2182,8 +2179,8 @@
       <c r="O30" s="43"/>
       <c r="P30" s="30"/>
       <c r="Q30" s="29"/>
-      <c r="R30" s="93"/>
-      <c r="S30" s="78"/>
+      <c r="R30" s="95"/>
+      <c r="S30" s="92"/>
       <c r="T30" s="43"/>
       <c r="U30" s="75"/>
       <c r="V30" s="76"/>
@@ -2215,8 +2212,8 @@
       <c r="O31" s="43"/>
       <c r="P31" s="30"/>
       <c r="Q31" s="29"/>
-      <c r="R31" s="93"/>
-      <c r="S31" s="78"/>
+      <c r="R31" s="95"/>
+      <c r="S31" s="92"/>
       <c r="T31" s="43"/>
       <c r="U31" s="75"/>
       <c r="V31" s="76"/>
@@ -2239,32 +2236,30 @@
       </c>
       <c r="G32" s="43"/>
       <c r="H32" s="43"/>
-      <c r="I32" s="75"/>
+      <c r="I32" s="89"/>
       <c r="J32" s="76"/>
       <c r="K32" s="43"/>
-      <c r="L32" s="33" t="s">
-        <v>36</v>
-      </c>
+      <c r="L32" s="29"/>
       <c r="M32" s="43"/>
-      <c r="N32" s="43"/>
+      <c r="N32" s="46"/>
       <c r="O32" s="43"/>
       <c r="P32" s="29"/>
       <c r="Q32" s="29"/>
-      <c r="R32" s="77"/>
-      <c r="S32" s="78"/>
+      <c r="R32" s="91"/>
+      <c r="S32" s="92"/>
       <c r="T32" s="43"/>
-      <c r="U32" s="75"/>
+      <c r="U32" s="89"/>
       <c r="V32" s="76"/>
       <c r="W32" s="75"/>
       <c r="X32" s="76"/>
-      <c r="Y32" s="43"/>
+      <c r="Y32" s="46"/>
       <c r="Z32" s="31"/>
     </row>
     <row r="33" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
       <c r="B33" s="52"/>
       <c r="C33" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>36</v>
@@ -2274,22 +2269,22 @@
       </c>
       <c r="G33" s="43"/>
       <c r="H33" s="43"/>
-      <c r="I33" s="89"/>
-      <c r="J33" s="76"/>
-      <c r="K33" s="43"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="45"/>
       <c r="L33" s="29"/>
-      <c r="M33" s="43"/>
+      <c r="M33" s="45"/>
       <c r="N33" s="46"/>
-      <c r="O33" s="43"/>
+      <c r="O33" s="45"/>
       <c r="P33" s="29"/>
       <c r="Q33" s="29"/>
-      <c r="R33" s="77"/>
-      <c r="S33" s="78"/>
+      <c r="R33" s="99"/>
+      <c r="S33" s="100"/>
       <c r="T33" s="43"/>
-      <c r="U33" s="89"/>
-      <c r="V33" s="76"/>
-      <c r="W33" s="75"/>
-      <c r="X33" s="76"/>
+      <c r="U33" s="46"/>
+      <c r="V33" s="45"/>
+      <c r="W33" s="83"/>
+      <c r="X33" s="84"/>
       <c r="Y33" s="46"/>
       <c r="Z33" s="31"/>
     </row>
@@ -2297,7 +2292,7 @@
       <c r="A34" s="9"/>
       <c r="B34" s="52"/>
       <c r="C34" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>36</v>
@@ -2309,86 +2304,86 @@
       <c r="H34" s="43"/>
       <c r="I34" s="35"/>
       <c r="J34" s="36"/>
-      <c r="K34" s="45"/>
+      <c r="K34" s="36"/>
       <c r="L34" s="29"/>
       <c r="M34" s="45"/>
       <c r="N34" s="46"/>
       <c r="O34" s="45"/>
       <c r="P34" s="29"/>
       <c r="Q34" s="29"/>
-      <c r="R34" s="95"/>
-      <c r="S34" s="96"/>
+      <c r="R34" s="97"/>
+      <c r="S34" s="98"/>
       <c r="T34" s="43"/>
       <c r="U34" s="46"/>
       <c r="V34" s="45"/>
-      <c r="W34" s="80"/>
-      <c r="X34" s="81"/>
+      <c r="W34" s="81"/>
+      <c r="X34" s="82"/>
       <c r="Y34" s="46"/>
       <c r="Z34" s="31"/>
     </row>
     <row r="35" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
-      <c r="B35" s="52"/>
-      <c r="C35" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="G35" s="43"/>
       <c r="H35" s="43"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="36"/>
+      <c r="I35" s="91"/>
+      <c r="J35" s="92"/>
+      <c r="K35" s="29"/>
       <c r="L35" s="29"/>
-      <c r="M35" s="45"/>
-      <c r="N35" s="46"/>
-      <c r="O35" s="45"/>
+      <c r="M35" s="43"/>
+      <c r="N35" s="43"/>
+      <c r="O35" s="43"/>
       <c r="P35" s="29"/>
       <c r="Q35" s="29"/>
       <c r="R35" s="91"/>
       <c r="S35" s="92"/>
       <c r="T35" s="43"/>
-      <c r="U35" s="46"/>
-      <c r="V35" s="45"/>
-      <c r="W35" s="82"/>
-      <c r="X35" s="83"/>
-      <c r="Y35" s="46"/>
-      <c r="Z35" s="31"/>
-    </row>
-    <row r="36" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="U35" s="75"/>
+      <c r="V35" s="76"/>
+      <c r="W35" s="75"/>
+      <c r="X35" s="76"/>
+      <c r="Y35" s="43"/>
+      <c r="Z35" s="29"/>
+    </row>
+    <row r="36" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
+      <c r="B36" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G36" s="43"/>
       <c r="H36" s="43"/>
-      <c r="I36" s="77"/>
-      <c r="J36" s="78"/>
+      <c r="I36" s="91"/>
+      <c r="J36" s="92"/>
       <c r="K36" s="29"/>
       <c r="L36" s="29"/>
       <c r="M36" s="43"/>
-      <c r="N36" s="43"/>
+      <c r="N36" s="42"/>
       <c r="O36" s="43"/>
       <c r="P36" s="29"/>
       <c r="Q36" s="29"/>
-      <c r="R36" s="77"/>
-      <c r="S36" s="78"/>
+      <c r="R36" s="91"/>
+      <c r="S36" s="92"/>
       <c r="T36" s="43"/>
-      <c r="U36" s="75"/>
+      <c r="U36" s="90"/>
       <c r="V36" s="76"/>
       <c r="W36" s="75"/>
       <c r="X36" s="76"/>
       <c r="Y36" s="43"/>
-      <c r="Z36" s="29"/>
-    </row>
-    <row r="37" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+      <c r="Z36" s="31"/>
+    </row>
+    <row r="37" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
-      <c r="B37" s="53" t="s">
-        <v>43</v>
-      </c>
+      <c r="B37" s="54"/>
       <c r="C37" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>23</v>
@@ -2398,30 +2393,30 @@
       </c>
       <c r="G37" s="43"/>
       <c r="H37" s="43"/>
-      <c r="I37" s="77"/>
-      <c r="J37" s="78"/>
+      <c r="I37" s="91"/>
+      <c r="J37" s="92"/>
       <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
+      <c r="L37" s="33"/>
       <c r="M37" s="43"/>
       <c r="N37" s="42"/>
       <c r="O37" s="43"/>
       <c r="P37" s="29"/>
       <c r="Q37" s="29"/>
-      <c r="R37" s="77"/>
-      <c r="S37" s="78"/>
-      <c r="T37" s="43"/>
+      <c r="R37" s="91"/>
+      <c r="S37" s="92"/>
+      <c r="T37" s="42"/>
       <c r="U37" s="90"/>
       <c r="V37" s="76"/>
       <c r="W37" s="75"/>
       <c r="X37" s="76"/>
-      <c r="Y37" s="43"/>
-      <c r="Z37" s="31"/>
+      <c r="Y37" s="42"/>
+      <c r="Z37" s="29"/>
     </row>
     <row r="38" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="9"/>
       <c r="B38" s="54"/>
       <c r="C38" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>23</v>
@@ -2431,30 +2426,30 @@
       </c>
       <c r="G38" s="43"/>
       <c r="H38" s="43"/>
-      <c r="I38" s="77"/>
-      <c r="J38" s="78"/>
+      <c r="I38" s="91"/>
+      <c r="J38" s="92"/>
       <c r="K38" s="29"/>
       <c r="L38" s="33"/>
       <c r="M38" s="43"/>
-      <c r="N38" s="42"/>
+      <c r="N38" s="43"/>
       <c r="O38" s="43"/>
       <c r="P38" s="29"/>
       <c r="Q38" s="29"/>
-      <c r="R38" s="77"/>
-      <c r="S38" s="78"/>
-      <c r="T38" s="42"/>
-      <c r="U38" s="90"/>
+      <c r="R38" s="91"/>
+      <c r="S38" s="92"/>
+      <c r="T38" s="43"/>
+      <c r="U38" s="75"/>
       <c r="V38" s="76"/>
       <c r="W38" s="75"/>
       <c r="X38" s="76"/>
-      <c r="Y38" s="42"/>
+      <c r="Y38" s="43"/>
       <c r="Z38" s="29"/>
     </row>
     <row r="39" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="54"/>
       <c r="C39" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>23</v>
@@ -2464,30 +2459,30 @@
       </c>
       <c r="G39" s="43"/>
       <c r="H39" s="43"/>
-      <c r="I39" s="77"/>
-      <c r="J39" s="78"/>
+      <c r="I39" s="91"/>
+      <c r="J39" s="92"/>
       <c r="K39" s="29"/>
       <c r="L39" s="33"/>
       <c r="M39" s="43"/>
-      <c r="N39" s="43"/>
+      <c r="N39" s="42"/>
       <c r="O39" s="43"/>
       <c r="P39" s="29"/>
       <c r="Q39" s="29"/>
-      <c r="R39" s="77"/>
-      <c r="S39" s="78"/>
-      <c r="T39" s="43"/>
-      <c r="U39" s="75"/>
+      <c r="R39" s="91"/>
+      <c r="S39" s="92"/>
+      <c r="T39" s="42"/>
+      <c r="U39" s="90"/>
       <c r="V39" s="76"/>
       <c r="W39" s="75"/>
       <c r="X39" s="76"/>
-      <c r="Y39" s="43"/>
-      <c r="Z39" s="29"/>
+      <c r="Y39" s="42"/>
+      <c r="Z39" s="31"/>
     </row>
     <row r="40" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="9"/>
       <c r="B40" s="54"/>
       <c r="C40" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>23</v>
@@ -2495,32 +2490,32 @@
       <c r="E40" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G40" s="43"/>
+      <c r="G40" s="40"/>
       <c r="H40" s="43"/>
-      <c r="I40" s="77"/>
-      <c r="J40" s="78"/>
+      <c r="I40" s="91"/>
+      <c r="J40" s="92"/>
       <c r="K40" s="29"/>
       <c r="L40" s="33"/>
       <c r="M40" s="43"/>
-      <c r="N40" s="42"/>
+      <c r="N40" s="40"/>
       <c r="O40" s="43"/>
-      <c r="P40" s="29"/>
+      <c r="P40" s="30"/>
       <c r="Q40" s="29"/>
-      <c r="R40" s="77"/>
-      <c r="S40" s="78"/>
-      <c r="T40" s="42"/>
-      <c r="U40" s="90"/>
+      <c r="R40" s="95"/>
+      <c r="S40" s="92"/>
+      <c r="T40" s="43"/>
+      <c r="U40" s="75"/>
       <c r="V40" s="76"/>
-      <c r="W40" s="75"/>
+      <c r="W40" s="79"/>
       <c r="X40" s="76"/>
-      <c r="Y40" s="42"/>
-      <c r="Z40" s="31"/>
+      <c r="Y40" s="40"/>
+      <c r="Z40" s="34"/>
     </row>
     <row r="41" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
       <c r="B41" s="54"/>
       <c r="C41" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>23</v>
@@ -2528,32 +2523,32 @@
       <c r="E41" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G41" s="40"/>
+      <c r="G41" s="43"/>
       <c r="H41" s="43"/>
-      <c r="I41" s="77"/>
-      <c r="J41" s="78"/>
+      <c r="I41" s="91"/>
+      <c r="J41" s="92"/>
       <c r="K41" s="29"/>
       <c r="L41" s="33"/>
       <c r="M41" s="43"/>
-      <c r="N41" s="40"/>
+      <c r="N41" s="42"/>
       <c r="O41" s="43"/>
-      <c r="P41" s="30"/>
+      <c r="P41" s="29"/>
       <c r="Q41" s="29"/>
-      <c r="R41" s="93"/>
-      <c r="S41" s="78"/>
+      <c r="R41" s="91"/>
+      <c r="S41" s="92"/>
       <c r="T41" s="43"/>
-      <c r="U41" s="75"/>
+      <c r="U41" s="90"/>
       <c r="V41" s="76"/>
-      <c r="W41" s="79"/>
+      <c r="W41" s="75"/>
       <c r="X41" s="76"/>
-      <c r="Y41" s="40"/>
-      <c r="Z41" s="34"/>
+      <c r="Y41" s="43"/>
+      <c r="Z41" s="31"/>
     </row>
     <row r="42" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="9"/>
       <c r="B42" s="54"/>
       <c r="C42" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>23</v>
@@ -2561,32 +2556,32 @@
       <c r="E42" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G42" s="43"/>
+      <c r="G42" s="40"/>
       <c r="H42" s="43"/>
-      <c r="I42" s="77"/>
-      <c r="J42" s="78"/>
+      <c r="I42" s="91"/>
+      <c r="J42" s="92"/>
       <c r="K42" s="29"/>
-      <c r="L42" s="33"/>
+      <c r="L42" s="29"/>
       <c r="M42" s="43"/>
-      <c r="N42" s="42"/>
+      <c r="N42" s="40"/>
       <c r="O42" s="43"/>
-      <c r="P42" s="29"/>
+      <c r="P42" s="30"/>
       <c r="Q42" s="29"/>
-      <c r="R42" s="77"/>
-      <c r="S42" s="78"/>
+      <c r="R42" s="79"/>
+      <c r="S42" s="76"/>
       <c r="T42" s="43"/>
-      <c r="U42" s="90"/>
+      <c r="U42" s="75"/>
       <c r="V42" s="76"/>
-      <c r="W42" s="75"/>
+      <c r="W42" s="79"/>
       <c r="X42" s="76"/>
-      <c r="Y42" s="43"/>
-      <c r="Z42" s="31"/>
+      <c r="Y42" s="40"/>
+      <c r="Z42" s="34"/>
     </row>
     <row r="43" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="9"/>
       <c r="B43" s="54"/>
       <c r="C43" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>23</v>
@@ -2596,8 +2591,8 @@
       </c>
       <c r="G43" s="40"/>
       <c r="H43" s="43"/>
-      <c r="I43" s="77"/>
-      <c r="J43" s="78"/>
+      <c r="I43" s="91"/>
+      <c r="J43" s="92"/>
       <c r="K43" s="29"/>
       <c r="L43" s="29"/>
       <c r="M43" s="43"/>
@@ -2619,7 +2614,7 @@
       <c r="A44" s="9"/>
       <c r="B44" s="54"/>
       <c r="C44" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>23</v>
@@ -2629,8 +2624,8 @@
       </c>
       <c r="G44" s="40"/>
       <c r="H44" s="43"/>
-      <c r="I44" s="77"/>
-      <c r="J44" s="78"/>
+      <c r="I44" s="91"/>
+      <c r="J44" s="92"/>
       <c r="K44" s="29"/>
       <c r="L44" s="29"/>
       <c r="M44" s="43"/>
@@ -2651,41 +2646,41 @@
     <row r="45" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
       <c r="B45" s="54"/>
-      <c r="C45" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>23</v>
+      <c r="C45" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G45" s="40"/>
+      <c r="G45" s="43"/>
       <c r="H45" s="43"/>
-      <c r="I45" s="77"/>
-      <c r="J45" s="78"/>
+      <c r="I45" s="104"/>
+      <c r="J45" s="92"/>
       <c r="K45" s="29"/>
       <c r="L45" s="29"/>
       <c r="M45" s="43"/>
-      <c r="N45" s="40"/>
+      <c r="N45" s="46"/>
       <c r="O45" s="43"/>
-      <c r="P45" s="30"/>
+      <c r="P45" s="29"/>
       <c r="Q45" s="29"/>
-      <c r="R45" s="79"/>
-      <c r="S45" s="76"/>
+      <c r="R45" s="91"/>
+      <c r="S45" s="92"/>
       <c r="T45" s="43"/>
-      <c r="U45" s="75"/>
+      <c r="U45" s="89"/>
       <c r="V45" s="76"/>
-      <c r="W45" s="79"/>
+      <c r="W45" s="75"/>
       <c r="X45" s="76"/>
-      <c r="Y45" s="40"/>
-      <c r="Z45" s="34"/>
+      <c r="Y45" s="46"/>
+      <c r="Z45" s="31"/>
     </row>
     <row r="46" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="9"/>
       <c r="B46" s="54"/>
       <c r="C46" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>36</v>
@@ -2695,23 +2690,23 @@
       </c>
       <c r="G46" s="43"/>
       <c r="H46" s="43"/>
-      <c r="I46" s="77"/>
-      <c r="J46" s="78"/>
-      <c r="K46" s="29"/>
-      <c r="L46" s="33"/>
-      <c r="M46" s="43"/>
-      <c r="N46" s="43"/>
-      <c r="O46" s="43"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="36"/>
+      <c r="K46" s="36"/>
+      <c r="L46" s="29"/>
+      <c r="M46" s="45"/>
+      <c r="N46" s="46"/>
+      <c r="O46" s="45"/>
       <c r="P46" s="29"/>
       <c r="Q46" s="29"/>
-      <c r="R46" s="77"/>
-      <c r="S46" s="78"/>
+      <c r="R46" s="99"/>
+      <c r="S46" s="100"/>
       <c r="T46" s="43"/>
-      <c r="U46" s="75"/>
-      <c r="V46" s="76"/>
-      <c r="W46" s="75"/>
-      <c r="X46" s="76"/>
-      <c r="Y46" s="43"/>
+      <c r="U46" s="46"/>
+      <c r="V46" s="45"/>
+      <c r="W46" s="77"/>
+      <c r="X46" s="78"/>
+      <c r="Y46" s="46"/>
       <c r="Z46" s="31"/>
     </row>
     <row r="47" spans="1:26" ht="16" x14ac:dyDescent="0.2">
@@ -2728,121 +2723,121 @@
       </c>
       <c r="G47" s="43"/>
       <c r="H47" s="43"/>
-      <c r="I47" s="100"/>
-      <c r="J47" s="78"/>
-      <c r="K47" s="29"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="36"/>
+      <c r="K47" s="36"/>
       <c r="L47" s="29"/>
-      <c r="M47" s="43"/>
+      <c r="M47" s="45"/>
       <c r="N47" s="46"/>
-      <c r="O47" s="43"/>
+      <c r="O47" s="45"/>
       <c r="P47" s="29"/>
       <c r="Q47" s="29"/>
-      <c r="R47" s="77"/>
-      <c r="S47" s="78"/>
+      <c r="R47" s="97"/>
+      <c r="S47" s="98"/>
       <c r="T47" s="43"/>
-      <c r="U47" s="89"/>
-      <c r="V47" s="76"/>
-      <c r="W47" s="75"/>
-      <c r="X47" s="76"/>
+      <c r="U47" s="46"/>
+      <c r="V47" s="45"/>
+      <c r="W47" s="77"/>
+      <c r="X47" s="78"/>
       <c r="Y47" s="46"/>
       <c r="Z47" s="31"/>
     </row>
     <row r="48" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="9"/>
-      <c r="B48" s="54"/>
-      <c r="C48" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="G48" s="43"/>
       <c r="H48" s="43"/>
-      <c r="I48" s="35"/>
-      <c r="J48" s="36"/>
-      <c r="K48" s="36"/>
+      <c r="I48" s="91"/>
+      <c r="J48" s="92"/>
+      <c r="K48" s="29"/>
       <c r="L48" s="29"/>
-      <c r="M48" s="45"/>
-      <c r="N48" s="46"/>
-      <c r="O48" s="45"/>
+      <c r="M48" s="43"/>
+      <c r="N48" s="43"/>
+      <c r="O48" s="43"/>
       <c r="P48" s="29"/>
       <c r="Q48" s="29"/>
-      <c r="R48" s="95"/>
-      <c r="S48" s="96"/>
+      <c r="R48" s="91"/>
+      <c r="S48" s="92"/>
       <c r="T48" s="43"/>
-      <c r="U48" s="46"/>
-      <c r="V48" s="45"/>
-      <c r="W48" s="107"/>
-      <c r="X48" s="108"/>
-      <c r="Y48" s="46"/>
-      <c r="Z48" s="31"/>
-    </row>
-    <row r="49" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="U48" s="75"/>
+      <c r="V48" s="76"/>
+      <c r="W48" s="75"/>
+      <c r="X48" s="76"/>
+      <c r="Y48" s="43"/>
+      <c r="Z48" s="29"/>
+    </row>
+    <row r="49" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
-      <c r="B49" s="54"/>
-      <c r="C49" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>36</v>
+      <c r="B49" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G49" s="43"/>
       <c r="H49" s="43"/>
-      <c r="I49" s="35"/>
-      <c r="J49" s="36"/>
-      <c r="K49" s="36"/>
+      <c r="I49" s="91"/>
+      <c r="J49" s="92"/>
+      <c r="K49" s="29"/>
       <c r="L49" s="29"/>
-      <c r="M49" s="45"/>
-      <c r="N49" s="46"/>
-      <c r="O49" s="45"/>
+      <c r="M49" s="43"/>
+      <c r="N49" s="42"/>
+      <c r="O49" s="43"/>
       <c r="P49" s="29"/>
       <c r="Q49" s="29"/>
       <c r="R49" s="91"/>
       <c r="S49" s="92"/>
       <c r="T49" s="43"/>
-      <c r="U49" s="46"/>
-      <c r="V49" s="45"/>
-      <c r="W49" s="107"/>
-      <c r="X49" s="108"/>
-      <c r="Y49" s="46"/>
+      <c r="U49" s="90"/>
+      <c r="V49" s="76"/>
+      <c r="W49" s="75"/>
+      <c r="X49" s="76"/>
+      <c r="Y49" s="43"/>
       <c r="Z49" s="31"/>
     </row>
     <row r="50" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="9"/>
+      <c r="B50" s="55"/>
+      <c r="C50" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G50" s="43"/>
       <c r="H50" s="43"/>
-      <c r="I50" s="77"/>
-      <c r="J50" s="78"/>
+      <c r="I50" s="91"/>
+      <c r="J50" s="92"/>
       <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
+      <c r="L50" s="33"/>
       <c r="M50" s="43"/>
-      <c r="N50" s="43"/>
+      <c r="N50" s="42"/>
       <c r="O50" s="43"/>
       <c r="P50" s="29"/>
       <c r="Q50" s="29"/>
-      <c r="R50" s="77"/>
-      <c r="S50" s="78"/>
-      <c r="T50" s="43"/>
-      <c r="U50" s="75"/>
+      <c r="R50" s="91"/>
+      <c r="S50" s="92"/>
+      <c r="T50" s="42"/>
+      <c r="U50" s="90"/>
       <c r="V50" s="76"/>
       <c r="W50" s="75"/>
       <c r="X50" s="76"/>
-      <c r="Y50" s="43"/>
+      <c r="Y50" s="42"/>
       <c r="Z50" s="29"/>
     </row>
-    <row r="51" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
-      <c r="B51" s="65" t="s">
-        <v>44</v>
-      </c>
+      <c r="B51" s="55"/>
       <c r="C51" s="6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>23</v>
@@ -2852,30 +2847,30 @@
       </c>
       <c r="G51" s="43"/>
       <c r="H51" s="43"/>
-      <c r="I51" s="77"/>
-      <c r="J51" s="78"/>
+      <c r="I51" s="91"/>
+      <c r="J51" s="92"/>
       <c r="K51" s="29"/>
-      <c r="L51" s="29"/>
+      <c r="L51" s="33"/>
       <c r="M51" s="43"/>
       <c r="N51" s="42"/>
       <c r="O51" s="43"/>
       <c r="P51" s="29"/>
       <c r="Q51" s="29"/>
-      <c r="R51" s="77"/>
-      <c r="S51" s="78"/>
-      <c r="T51" s="43"/>
+      <c r="R51" s="91"/>
+      <c r="S51" s="92"/>
+      <c r="T51" s="42"/>
       <c r="U51" s="90"/>
       <c r="V51" s="76"/>
       <c r="W51" s="75"/>
       <c r="X51" s="76"/>
-      <c r="Y51" s="43"/>
+      <c r="Y51" s="42"/>
       <c r="Z51" s="31"/>
     </row>
     <row r="52" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="9"/>
       <c r="B52" s="55"/>
       <c r="C52" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>23</v>
@@ -2883,32 +2878,32 @@
       <c r="E52" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G52" s="43"/>
+      <c r="G52" s="40"/>
       <c r="H52" s="43"/>
-      <c r="I52" s="77"/>
-      <c r="J52" s="78"/>
+      <c r="I52" s="91"/>
+      <c r="J52" s="92"/>
       <c r="K52" s="29"/>
       <c r="L52" s="33"/>
       <c r="M52" s="43"/>
-      <c r="N52" s="42"/>
+      <c r="N52" s="40"/>
       <c r="O52" s="43"/>
-      <c r="P52" s="29"/>
+      <c r="P52" s="30"/>
       <c r="Q52" s="29"/>
-      <c r="R52" s="77"/>
-      <c r="S52" s="78"/>
-      <c r="T52" s="42"/>
-      <c r="U52" s="90"/>
+      <c r="R52" s="95"/>
+      <c r="S52" s="92"/>
+      <c r="T52" s="43"/>
+      <c r="U52" s="75"/>
       <c r="V52" s="76"/>
-      <c r="W52" s="75"/>
+      <c r="W52" s="79"/>
       <c r="X52" s="76"/>
-      <c r="Y52" s="42"/>
-      <c r="Z52" s="29"/>
+      <c r="Y52" s="40"/>
+      <c r="Z52" s="34"/>
     </row>
     <row r="53" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="9"/>
       <c r="B53" s="55"/>
       <c r="C53" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>23</v>
@@ -2918,8 +2913,8 @@
       </c>
       <c r="G53" s="43"/>
       <c r="H53" s="43"/>
-      <c r="I53" s="77"/>
-      <c r="J53" s="78"/>
+      <c r="I53" s="91"/>
+      <c r="J53" s="92"/>
       <c r="K53" s="29"/>
       <c r="L53" s="33"/>
       <c r="M53" s="43"/>
@@ -2927,8 +2922,8 @@
       <c r="O53" s="43"/>
       <c r="P53" s="29"/>
       <c r="Q53" s="29"/>
-      <c r="R53" s="77"/>
-      <c r="S53" s="78"/>
+      <c r="R53" s="91"/>
+      <c r="S53" s="92"/>
       <c r="T53" s="42"/>
       <c r="U53" s="90"/>
       <c r="V53" s="76"/>
@@ -2941,7 +2936,7 @@
       <c r="A54" s="9"/>
       <c r="B54" s="55"/>
       <c r="C54" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>23</v>
@@ -2951,17 +2946,17 @@
       </c>
       <c r="G54" s="40"/>
       <c r="H54" s="43"/>
-      <c r="I54" s="77"/>
-      <c r="J54" s="78"/>
+      <c r="I54" s="91"/>
+      <c r="J54" s="92"/>
       <c r="K54" s="29"/>
-      <c r="L54" s="33"/>
+      <c r="L54" s="29"/>
       <c r="M54" s="43"/>
       <c r="N54" s="40"/>
       <c r="O54" s="43"/>
       <c r="P54" s="30"/>
       <c r="Q54" s="29"/>
-      <c r="R54" s="93"/>
-      <c r="S54" s="78"/>
+      <c r="R54" s="95"/>
+      <c r="S54" s="92"/>
       <c r="T54" s="43"/>
       <c r="U54" s="75"/>
       <c r="V54" s="76"/>
@@ -2974,7 +2969,7 @@
       <c r="A55" s="9"/>
       <c r="B55" s="55"/>
       <c r="C55" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>23</v>
@@ -2982,32 +2977,32 @@
       <c r="E55" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G55" s="43"/>
+      <c r="G55" s="40"/>
       <c r="H55" s="43"/>
-      <c r="I55" s="77"/>
-      <c r="J55" s="78"/>
+      <c r="I55" s="91"/>
+      <c r="J55" s="92"/>
       <c r="K55" s="29"/>
-      <c r="L55" s="33"/>
+      <c r="L55" s="29"/>
       <c r="M55" s="43"/>
-      <c r="N55" s="42"/>
+      <c r="N55" s="40"/>
       <c r="O55" s="43"/>
-      <c r="P55" s="29"/>
+      <c r="P55" s="30"/>
       <c r="Q55" s="29"/>
-      <c r="R55" s="77"/>
-      <c r="S55" s="78"/>
-      <c r="T55" s="42"/>
-      <c r="U55" s="90"/>
+      <c r="R55" s="95"/>
+      <c r="S55" s="92"/>
+      <c r="T55" s="43"/>
+      <c r="U55" s="75"/>
       <c r="V55" s="76"/>
-      <c r="W55" s="75"/>
+      <c r="W55" s="79"/>
       <c r="X55" s="76"/>
-      <c r="Y55" s="42"/>
-      <c r="Z55" s="31"/>
+      <c r="Y55" s="40"/>
+      <c r="Z55" s="34"/>
     </row>
     <row r="56" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="9"/>
       <c r="B56" s="55"/>
-      <c r="C56" s="6" t="s">
-        <v>31</v>
+      <c r="C56" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>23</v>
@@ -3017,90 +3012,90 @@
       </c>
       <c r="G56" s="40"/>
       <c r="H56" s="43"/>
-      <c r="I56" s="77"/>
-      <c r="J56" s="78"/>
-      <c r="K56" s="29"/>
+      <c r="I56" s="96"/>
+      <c r="J56" s="92"/>
+      <c r="K56" s="36"/>
       <c r="L56" s="29"/>
-      <c r="M56" s="43"/>
+      <c r="M56" s="45"/>
       <c r="N56" s="40"/>
-      <c r="O56" s="43"/>
+      <c r="O56" s="45"/>
       <c r="P56" s="30"/>
       <c r="Q56" s="29"/>
-      <c r="R56" s="93"/>
-      <c r="S56" s="78"/>
+      <c r="R56" s="30"/>
+      <c r="S56" s="36"/>
       <c r="T56" s="43"/>
-      <c r="U56" s="75"/>
+      <c r="U56" s="80"/>
       <c r="V56" s="76"/>
-      <c r="W56" s="79"/>
-      <c r="X56" s="76"/>
+      <c r="W56" s="40"/>
+      <c r="X56" s="45"/>
       <c r="Y56" s="40"/>
       <c r="Z56" s="34"/>
     </row>
     <row r="57" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="9"/>
       <c r="B57" s="55"/>
-      <c r="C57" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>23</v>
+      <c r="C57" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G57" s="40"/>
+      <c r="G57" s="43"/>
       <c r="H57" s="43"/>
-      <c r="I57" s="77"/>
-      <c r="J57" s="78"/>
+      <c r="I57" s="104"/>
+      <c r="J57" s="92"/>
       <c r="K57" s="29"/>
       <c r="L57" s="29"/>
       <c r="M57" s="43"/>
-      <c r="N57" s="40"/>
+      <c r="N57" s="46"/>
       <c r="O57" s="43"/>
-      <c r="P57" s="30"/>
+      <c r="P57" s="29"/>
       <c r="Q57" s="29"/>
-      <c r="R57" s="93"/>
-      <c r="S57" s="78"/>
+      <c r="R57" s="91"/>
+      <c r="S57" s="92"/>
       <c r="T57" s="43"/>
-      <c r="U57" s="75"/>
+      <c r="U57" s="89"/>
       <c r="V57" s="76"/>
-      <c r="W57" s="79"/>
+      <c r="W57" s="75"/>
       <c r="X57" s="76"/>
-      <c r="Y57" s="40"/>
-      <c r="Z57" s="34"/>
+      <c r="Y57" s="46"/>
+      <c r="Z57" s="31"/>
     </row>
     <row r="58" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="9"/>
       <c r="B58" s="55"/>
       <c r="C58" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G58" s="40"/>
+      <c r="G58" s="43"/>
       <c r="H58" s="43"/>
-      <c r="I58" s="94"/>
-      <c r="J58" s="78"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="36"/>
       <c r="K58" s="36"/>
       <c r="L58" s="29"/>
       <c r="M58" s="45"/>
-      <c r="N58" s="40"/>
+      <c r="N58" s="46"/>
       <c r="O58" s="45"/>
-      <c r="P58" s="30"/>
+      <c r="P58" s="29"/>
       <c r="Q58" s="29"/>
-      <c r="R58" s="30"/>
-      <c r="S58" s="36"/>
+      <c r="R58" s="96"/>
+      <c r="S58" s="92"/>
       <c r="T58" s="43"/>
-      <c r="U58" s="84"/>
-      <c r="V58" s="76"/>
-      <c r="W58" s="40"/>
-      <c r="X58" s="45"/>
-      <c r="Y58" s="40"/>
-      <c r="Z58" s="34"/>
+      <c r="U58" s="46"/>
+      <c r="V58" s="45"/>
+      <c r="W58" s="80"/>
+      <c r="X58" s="76"/>
+      <c r="Y58" s="46"/>
+      <c r="Z58" s="31"/>
     </row>
     <row r="59" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="9"/>
@@ -3116,8 +3111,8 @@
       </c>
       <c r="G59" s="43"/>
       <c r="H59" s="43"/>
-      <c r="I59" s="100"/>
-      <c r="J59" s="78"/>
+      <c r="I59" s="104"/>
+      <c r="J59" s="92"/>
       <c r="K59" s="29"/>
       <c r="L59" s="29"/>
       <c r="M59" s="43"/>
@@ -3125,8 +3120,8 @@
       <c r="O59" s="43"/>
       <c r="P59" s="29"/>
       <c r="Q59" s="29"/>
-      <c r="R59" s="77"/>
-      <c r="S59" s="78"/>
+      <c r="R59" s="91"/>
+      <c r="S59" s="92"/>
       <c r="T59" s="43"/>
       <c r="U59" s="89"/>
       <c r="V59" s="76"/>
@@ -3137,325 +3132,323 @@
     </row>
     <row r="60" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="9"/>
-      <c r="B60" s="55"/>
-      <c r="C60" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="C60" s="6"/>
       <c r="G60" s="43"/>
       <c r="H60" s="43"/>
-      <c r="I60" s="35"/>
-      <c r="J60" s="36"/>
-      <c r="K60" s="36"/>
+      <c r="I60" s="91"/>
+      <c r="J60" s="92"/>
+      <c r="K60" s="29"/>
       <c r="L60" s="29"/>
-      <c r="M60" s="45"/>
-      <c r="N60" s="46"/>
-      <c r="O60" s="45"/>
+      <c r="M60" s="43"/>
+      <c r="N60" s="43"/>
+      <c r="O60" s="43"/>
       <c r="P60" s="29"/>
       <c r="Q60" s="29"/>
-      <c r="R60" s="94"/>
-      <c r="S60" s="78"/>
+      <c r="R60" s="91"/>
+      <c r="S60" s="92"/>
       <c r="T60" s="43"/>
-      <c r="U60" s="46"/>
-      <c r="V60" s="45"/>
-      <c r="W60" s="84"/>
+      <c r="U60" s="75"/>
+      <c r="V60" s="76"/>
+      <c r="W60" s="75"/>
       <c r="X60" s="76"/>
-      <c r="Y60" s="46"/>
+      <c r="Y60" s="43"/>
       <c r="Z60" s="31"/>
     </row>
-    <row r="61" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="9"/>
-      <c r="B61" s="55"/>
-      <c r="C61" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>36</v>
+      <c r="B61" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G61" s="43"/>
+        <v>46</v>
+      </c>
+      <c r="G61" s="40"/>
       <c r="H61" s="43"/>
-      <c r="I61" s="100"/>
-      <c r="J61" s="78"/>
+      <c r="I61" s="91"/>
+      <c r="J61" s="92"/>
       <c r="K61" s="29"/>
       <c r="L61" s="29"/>
       <c r="M61" s="43"/>
-      <c r="N61" s="46"/>
+      <c r="N61" s="40"/>
       <c r="O61" s="43"/>
-      <c r="P61" s="29"/>
+      <c r="P61" s="30"/>
       <c r="Q61" s="29"/>
-      <c r="R61" s="77"/>
-      <c r="S61" s="78"/>
+      <c r="R61" s="79"/>
+      <c r="S61" s="76"/>
       <c r="T61" s="43"/>
-      <c r="U61" s="89"/>
+      <c r="U61" s="75"/>
       <c r="V61" s="76"/>
-      <c r="W61" s="75"/>
+      <c r="W61" s="79"/>
       <c r="X61" s="76"/>
-      <c r="Y61" s="46"/>
-      <c r="Z61" s="31"/>
+      <c r="Y61" s="40"/>
+      <c r="Z61" s="34"/>
     </row>
     <row r="62" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="9"/>
-      <c r="C62" s="6"/>
-      <c r="G62" s="43"/>
+      <c r="B62" s="56"/>
+      <c r="C62" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G62" s="40"/>
       <c r="H62" s="43"/>
-      <c r="I62" s="77"/>
-      <c r="J62" s="78"/>
+      <c r="I62" s="91"/>
+      <c r="J62" s="92"/>
       <c r="K62" s="29"/>
       <c r="L62" s="29"/>
       <c r="M62" s="43"/>
-      <c r="N62" s="43"/>
+      <c r="N62" s="40"/>
       <c r="O62" s="43"/>
-      <c r="P62" s="29"/>
+      <c r="P62" s="30"/>
       <c r="Q62" s="29"/>
-      <c r="R62" s="77"/>
-      <c r="S62" s="78"/>
+      <c r="R62" s="95"/>
+      <c r="S62" s="92"/>
       <c r="T62" s="43"/>
       <c r="U62" s="75"/>
       <c r="V62" s="76"/>
-      <c r="W62" s="75"/>
+      <c r="W62" s="79"/>
       <c r="X62" s="76"/>
-      <c r="Y62" s="43"/>
-      <c r="Z62" s="31"/>
-    </row>
-    <row r="63" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+      <c r="Y62" s="40"/>
+      <c r="Z62" s="34"/>
+    </row>
+    <row r="63" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="9"/>
-      <c r="B63" s="64" t="s">
+      <c r="B63" s="56"/>
+      <c r="C63" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="G63" s="40"/>
       <c r="H63" s="43"/>
-      <c r="I63" s="77"/>
-      <c r="J63" s="78"/>
-      <c r="K63" s="29"/>
+      <c r="I63" s="99"/>
+      <c r="J63" s="100"/>
+      <c r="K63" s="36"/>
       <c r="L63" s="29"/>
-      <c r="M63" s="43"/>
+      <c r="M63" s="45"/>
       <c r="N63" s="40"/>
-      <c r="O63" s="43"/>
+      <c r="O63" s="45"/>
       <c r="P63" s="30"/>
       <c r="Q63" s="29"/>
-      <c r="R63" s="79"/>
-      <c r="S63" s="76"/>
+      <c r="R63" s="30"/>
+      <c r="S63" s="36"/>
       <c r="T63" s="43"/>
-      <c r="U63" s="75"/>
-      <c r="V63" s="76"/>
-      <c r="W63" s="79"/>
-      <c r="X63" s="76"/>
+      <c r="U63" s="77"/>
+      <c r="V63" s="78"/>
+      <c r="W63" s="40"/>
+      <c r="X63" s="45"/>
       <c r="Y63" s="40"/>
       <c r="Z63" s="34"/>
     </row>
     <row r="64" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="9"/>
       <c r="B64" s="56"/>
-      <c r="C64" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G64" s="40"/>
-      <c r="H64" s="43"/>
-      <c r="I64" s="77"/>
-      <c r="J64" s="78"/>
-      <c r="K64" s="29"/>
-      <c r="L64" s="29"/>
-      <c r="M64" s="43"/>
-      <c r="N64" s="40"/>
-      <c r="O64" s="43"/>
-      <c r="P64" s="30"/>
-      <c r="Q64" s="29"/>
-      <c r="R64" s="93"/>
+      <c r="C64" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F64" s="10"/>
+      <c r="G64" s="43"/>
+      <c r="H64" s="44"/>
+      <c r="I64" s="105"/>
+      <c r="J64" s="106"/>
+      <c r="K64" s="36"/>
+      <c r="L64" s="37"/>
+      <c r="M64" s="45"/>
+      <c r="N64" s="44"/>
+      <c r="O64" s="45"/>
+      <c r="P64" s="29"/>
+      <c r="Q64" s="37"/>
+      <c r="R64" s="77"/>
       <c r="S64" s="78"/>
-      <c r="T64" s="43"/>
-      <c r="U64" s="75"/>
-      <c r="V64" s="76"/>
-      <c r="W64" s="79"/>
-      <c r="X64" s="76"/>
-      <c r="Y64" s="40"/>
-      <c r="Z64" s="34"/>
+      <c r="T64" s="44"/>
+      <c r="U64" s="77"/>
+      <c r="V64" s="78"/>
+      <c r="W64" s="77"/>
+      <c r="X64" s="78"/>
+      <c r="Y64" s="44"/>
+      <c r="Z64" s="31"/>
     </row>
     <row r="65" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="9"/>
       <c r="B65" s="56"/>
       <c r="C65" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G65" s="40"/>
+        <v>46</v>
+      </c>
+      <c r="G65" s="43"/>
       <c r="H65" s="43"/>
-      <c r="I65" s="95"/>
-      <c r="J65" s="96"/>
+      <c r="I65" s="97"/>
+      <c r="J65" s="98"/>
       <c r="K65" s="36"/>
       <c r="L65" s="29"/>
-      <c r="M65" s="45"/>
-      <c r="N65" s="40"/>
+      <c r="M65" s="36"/>
+      <c r="N65" s="43"/>
       <c r="O65" s="45"/>
-      <c r="P65" s="30"/>
+      <c r="P65" s="29"/>
       <c r="Q65" s="29"/>
-      <c r="R65" s="30"/>
-      <c r="S65" s="36"/>
+      <c r="R65" s="93"/>
+      <c r="S65" s="94"/>
       <c r="T65" s="43"/>
-      <c r="U65" s="107"/>
-      <c r="V65" s="108"/>
-      <c r="W65" s="40"/>
-      <c r="X65" s="45"/>
-      <c r="Y65" s="40"/>
-      <c r="Z65" s="34"/>
+      <c r="U65" s="77"/>
+      <c r="V65" s="78"/>
+      <c r="W65" s="77"/>
+      <c r="X65" s="78"/>
+      <c r="Y65" s="43"/>
+      <c r="Z65" s="31"/>
     </row>
     <row r="66" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="9"/>
-      <c r="B66" s="56"/>
-      <c r="C66" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E66" s="10" t="s">
+      <c r="G66" s="43"/>
+      <c r="H66" s="43"/>
+      <c r="I66" s="91"/>
+      <c r="J66" s="92"/>
+      <c r="K66" s="29"/>
+      <c r="L66" s="29"/>
+      <c r="M66" s="29"/>
+      <c r="N66" s="43"/>
+      <c r="O66" s="43"/>
+      <c r="P66" s="29"/>
+      <c r="Q66" s="29"/>
+      <c r="R66" s="91"/>
+      <c r="S66" s="92"/>
+      <c r="T66" s="43"/>
+      <c r="U66" s="75"/>
+      <c r="V66" s="76"/>
+      <c r="W66" s="75"/>
+      <c r="X66" s="76"/>
+      <c r="Y66" s="43"/>
+      <c r="Z66" s="31"/>
+    </row>
+    <row r="67" spans="1:26" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A67" s="12"/>
+      <c r="B67" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="F66" s="10"/>
-      <c r="G66" s="43"/>
-      <c r="H66" s="44"/>
-      <c r="I66" s="101"/>
-      <c r="J66" s="102"/>
-      <c r="K66" s="36"/>
-      <c r="L66" s="37"/>
-      <c r="M66" s="45"/>
-      <c r="N66" s="44"/>
-      <c r="O66" s="45"/>
-      <c r="P66" s="29"/>
-      <c r="Q66" s="37"/>
-      <c r="R66" s="107"/>
-      <c r="S66" s="108"/>
-      <c r="T66" s="44"/>
-      <c r="U66" s="107"/>
-      <c r="V66" s="108"/>
-      <c r="W66" s="107"/>
-      <c r="X66" s="108"/>
-      <c r="Y66" s="44"/>
-      <c r="Z66" s="31"/>
-    </row>
-    <row r="67" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="9"/>
-      <c r="B67" s="56"/>
-      <c r="C67" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="C67" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F67" s="14"/>
       <c r="G67" s="43"/>
       <c r="H67" s="43"/>
       <c r="I67" s="91"/>
       <c r="J67" s="92"/>
-      <c r="K67" s="36"/>
+      <c r="K67" s="29"/>
       <c r="L67" s="29"/>
-      <c r="M67" s="36"/>
-      <c r="N67" s="43"/>
-      <c r="O67" s="45"/>
+      <c r="M67" s="29"/>
+      <c r="N67" s="42"/>
+      <c r="O67" s="43"/>
       <c r="P67" s="29"/>
       <c r="Q67" s="29"/>
-      <c r="R67" s="109"/>
-      <c r="S67" s="110"/>
+      <c r="R67" s="91"/>
+      <c r="S67" s="92"/>
       <c r="T67" s="43"/>
-      <c r="U67" s="107"/>
-      <c r="V67" s="108"/>
-      <c r="W67" s="107"/>
-      <c r="X67" s="108"/>
+      <c r="U67" s="90"/>
+      <c r="V67" s="76"/>
+      <c r="W67" s="75"/>
+      <c r="X67" s="76"/>
       <c r="Y67" s="43"/>
       <c r="Z67" s="31"/>
     </row>
     <row r="68" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="9"/>
+      <c r="C68" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G68" s="43"/>
       <c r="H68" s="43"/>
-      <c r="I68" s="77"/>
-      <c r="J68" s="78"/>
+      <c r="I68" s="91"/>
+      <c r="J68" s="92"/>
       <c r="K68" s="29"/>
       <c r="L68" s="29"/>
       <c r="M68" s="29"/>
-      <c r="N68" s="43"/>
+      <c r="N68" s="42"/>
       <c r="O68" s="43"/>
       <c r="P68" s="29"/>
       <c r="Q68" s="29"/>
-      <c r="R68" s="77"/>
-      <c r="S68" s="78"/>
-      <c r="T68" s="43"/>
-      <c r="U68" s="75"/>
+      <c r="R68" s="91"/>
+      <c r="S68" s="92"/>
+      <c r="T68" s="42"/>
+      <c r="U68" s="90"/>
       <c r="V68" s="76"/>
       <c r="W68" s="75"/>
       <c r="X68" s="76"/>
-      <c r="Y68" s="43"/>
+      <c r="Y68" s="42"/>
       <c r="Z68" s="31"/>
     </row>
-    <row r="69" spans="1:26" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A69" s="12"/>
-      <c r="B69" s="63" t="s">
-        <v>48</v>
-      </c>
-      <c r="C69" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D69" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E69" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F69" s="14"/>
+    <row r="69" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="9"/>
+      <c r="C69" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G69" s="43"/>
       <c r="H69" s="43"/>
-      <c r="I69" s="77"/>
-      <c r="J69" s="78"/>
-      <c r="K69" s="29"/>
+      <c r="I69" s="91"/>
+      <c r="J69" s="92"/>
+      <c r="K69" s="38"/>
       <c r="L69" s="29"/>
-      <c r="M69" s="29"/>
+      <c r="M69" s="38"/>
       <c r="N69" s="42"/>
       <c r="O69" s="43"/>
       <c r="P69" s="29"/>
       <c r="Q69" s="29"/>
-      <c r="R69" s="77"/>
-      <c r="S69" s="78"/>
-      <c r="T69" s="43"/>
+      <c r="R69" s="91"/>
+      <c r="S69" s="92"/>
+      <c r="T69" s="42"/>
       <c r="U69" s="90"/>
       <c r="V69" s="76"/>
       <c r="W69" s="75"/>
       <c r="X69" s="76"/>
-      <c r="Y69" s="43"/>
+      <c r="Y69" s="42"/>
       <c r="Z69" s="31"/>
     </row>
     <row r="70" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="9"/>
       <c r="C70" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>23</v>
@@ -3465,8 +3458,8 @@
       </c>
       <c r="G70" s="43"/>
       <c r="H70" s="43"/>
-      <c r="I70" s="77"/>
-      <c r="J70" s="78"/>
+      <c r="I70" s="91"/>
+      <c r="J70" s="92"/>
       <c r="K70" s="29"/>
       <c r="L70" s="29"/>
       <c r="M70" s="29"/>
@@ -3474,8 +3467,8 @@
       <c r="O70" s="43"/>
       <c r="P70" s="29"/>
       <c r="Q70" s="29"/>
-      <c r="R70" s="77"/>
-      <c r="S70" s="78"/>
+      <c r="R70" s="91"/>
+      <c r="S70" s="92"/>
       <c r="T70" s="42"/>
       <c r="U70" s="90"/>
       <c r="V70" s="76"/>
@@ -3487,7 +3480,7 @@
     <row r="71" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="9"/>
       <c r="C71" s="6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>23</v>
@@ -3497,119 +3490,123 @@
       </c>
       <c r="G71" s="43"/>
       <c r="H71" s="43"/>
-      <c r="I71" s="77"/>
-      <c r="J71" s="78"/>
+      <c r="I71" s="91"/>
+      <c r="J71" s="92"/>
       <c r="K71" s="38"/>
       <c r="L71" s="29"/>
       <c r="M71" s="38"/>
-      <c r="N71" s="42"/>
+      <c r="N71" s="40"/>
       <c r="O71" s="43"/>
       <c r="P71" s="29"/>
       <c r="Q71" s="29"/>
-      <c r="R71" s="77"/>
-      <c r="S71" s="78"/>
-      <c r="T71" s="42"/>
-      <c r="U71" s="90"/>
+      <c r="R71" s="91"/>
+      <c r="S71" s="92"/>
+      <c r="T71" s="43"/>
+      <c r="U71" s="75"/>
       <c r="V71" s="76"/>
-      <c r="W71" s="75"/>
+      <c r="W71" s="79"/>
       <c r="X71" s="76"/>
-      <c r="Y71" s="42"/>
+      <c r="Y71" s="43"/>
       <c r="Z71" s="31"/>
     </row>
     <row r="72" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="9"/>
-      <c r="C72" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="C72" s="6"/>
       <c r="G72" s="43"/>
       <c r="H72" s="43"/>
-      <c r="I72" s="77"/>
-      <c r="J72" s="78"/>
+      <c r="I72" s="91"/>
+      <c r="J72" s="92"/>
       <c r="K72" s="29"/>
       <c r="L72" s="29"/>
       <c r="M72" s="29"/>
-      <c r="N72" s="42"/>
+      <c r="N72" s="43"/>
       <c r="O72" s="43"/>
       <c r="P72" s="29"/>
       <c r="Q72" s="29"/>
-      <c r="R72" s="77"/>
-      <c r="S72" s="78"/>
-      <c r="T72" s="42"/>
-      <c r="U72" s="90"/>
+      <c r="R72" s="91"/>
+      <c r="S72" s="92"/>
+      <c r="T72" s="43"/>
+      <c r="U72" s="75"/>
       <c r="V72" s="76"/>
       <c r="W72" s="75"/>
       <c r="X72" s="76"/>
-      <c r="Y72" s="42"/>
+      <c r="Y72" s="43"/>
       <c r="Z72" s="31"/>
     </row>
-    <row r="73" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A73" s="9"/>
-      <c r="C73" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="B73" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F73" s="10"/>
       <c r="G73" s="43"/>
-      <c r="H73" s="43"/>
-      <c r="I73" s="77"/>
-      <c r="J73" s="78"/>
-      <c r="K73" s="38"/>
-      <c r="L73" s="29"/>
-      <c r="M73" s="38"/>
-      <c r="N73" s="40"/>
-      <c r="O73" s="43"/>
+      <c r="H73" s="44"/>
+      <c r="I73" s="104"/>
+      <c r="J73" s="92"/>
+      <c r="K73" s="37"/>
+      <c r="L73" s="37"/>
+      <c r="M73" s="37"/>
+      <c r="N73" s="46"/>
+      <c r="O73" s="44"/>
       <c r="P73" s="29"/>
-      <c r="Q73" s="29"/>
-      <c r="R73" s="77"/>
-      <c r="S73" s="78"/>
-      <c r="T73" s="43"/>
-      <c r="U73" s="75"/>
+      <c r="Q73" s="37"/>
+      <c r="R73" s="91"/>
+      <c r="S73" s="92"/>
+      <c r="T73" s="44"/>
+      <c r="U73" s="89"/>
       <c r="V73" s="76"/>
-      <c r="W73" s="79"/>
+      <c r="W73" s="75"/>
       <c r="X73" s="76"/>
-      <c r="Y73" s="43"/>
-      <c r="Z73" s="31"/>
+      <c r="Y73" s="46"/>
+      <c r="Z73" s="29"/>
     </row>
     <row r="74" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="9"/>
-      <c r="C74" s="6"/>
+      <c r="B74" s="61"/>
+      <c r="C74" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F74" s="10"/>
       <c r="G74" s="43"/>
-      <c r="H74" s="43"/>
-      <c r="I74" s="77"/>
-      <c r="J74" s="78"/>
-      <c r="K74" s="29"/>
-      <c r="L74" s="29"/>
-      <c r="M74" s="29"/>
-      <c r="N74" s="43"/>
-      <c r="O74" s="43"/>
+      <c r="H74" s="44"/>
+      <c r="I74" s="104"/>
+      <c r="J74" s="92"/>
+      <c r="K74" s="37"/>
+      <c r="L74" s="37"/>
+      <c r="M74" s="37"/>
+      <c r="N74" s="46"/>
+      <c r="O74" s="44"/>
       <c r="P74" s="29"/>
-      <c r="Q74" s="29"/>
-      <c r="R74" s="77"/>
-      <c r="S74" s="78"/>
-      <c r="T74" s="43"/>
-      <c r="U74" s="75"/>
+      <c r="Q74" s="37"/>
+      <c r="R74" s="91"/>
+      <c r="S74" s="92"/>
+      <c r="T74" s="44"/>
+      <c r="U74" s="89"/>
       <c r="V74" s="76"/>
       <c r="W74" s="75"/>
       <c r="X74" s="76"/>
-      <c r="Y74" s="43"/>
-      <c r="Z74" s="31"/>
-    </row>
-    <row r="75" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+      <c r="Y74" s="46"/>
+      <c r="Z74" s="29"/>
+    </row>
+    <row r="75" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="9"/>
-      <c r="B75" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="C75" s="10" t="s">
+      <c r="B75" s="61"/>
+      <c r="C75" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D75" s="10" t="s">
@@ -3621,8 +3618,8 @@
       <c r="F75" s="10"/>
       <c r="G75" s="43"/>
       <c r="H75" s="44"/>
-      <c r="I75" s="100"/>
-      <c r="J75" s="78"/>
+      <c r="I75" s="104"/>
+      <c r="J75" s="92"/>
       <c r="K75" s="37"/>
       <c r="L75" s="37"/>
       <c r="M75" s="37"/>
@@ -3630,8 +3627,8 @@
       <c r="O75" s="44"/>
       <c r="P75" s="29"/>
       <c r="Q75" s="37"/>
-      <c r="R75" s="77"/>
-      <c r="S75" s="78"/>
+      <c r="R75" s="91"/>
+      <c r="S75" s="92"/>
       <c r="T75" s="44"/>
       <c r="U75" s="89"/>
       <c r="V75" s="76"/>
@@ -3642,87 +3639,87 @@
     </row>
     <row r="76" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="9"/>
-      <c r="B76" s="61"/>
-      <c r="C76" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D76" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E76" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F76" s="10"/>
       <c r="G76" s="43"/>
-      <c r="H76" s="44"/>
-      <c r="I76" s="100"/>
-      <c r="J76" s="78"/>
-      <c r="K76" s="37"/>
-      <c r="L76" s="37"/>
-      <c r="M76" s="37"/>
-      <c r="N76" s="46"/>
-      <c r="O76" s="44"/>
+      <c r="H76" s="43"/>
+      <c r="I76" s="91"/>
+      <c r="J76" s="92"/>
+      <c r="K76" s="29"/>
+      <c r="L76" s="29"/>
+      <c r="M76" s="29"/>
+      <c r="N76" s="43"/>
+      <c r="O76" s="43"/>
       <c r="P76" s="29"/>
-      <c r="Q76" s="37"/>
-      <c r="R76" s="77"/>
-      <c r="S76" s="78"/>
-      <c r="T76" s="44"/>
-      <c r="U76" s="89"/>
+      <c r="Q76" s="29"/>
+      <c r="R76" s="91"/>
+      <c r="S76" s="92"/>
+      <c r="T76" s="43"/>
+      <c r="U76" s="75"/>
       <c r="V76" s="76"/>
       <c r="W76" s="75"/>
       <c r="X76" s="76"/>
-      <c r="Y76" s="46"/>
+      <c r="Y76" s="43"/>
       <c r="Z76" s="29"/>
     </row>
-    <row r="77" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A77" s="9"/>
-      <c r="B77" s="61"/>
+      <c r="B77" s="60" t="s">
+        <v>55</v>
+      </c>
       <c r="C77" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D77" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F77" s="10"/>
+        <v>49</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G77" s="43"/>
-      <c r="H77" s="44"/>
-      <c r="I77" s="100"/>
-      <c r="J77" s="78"/>
-      <c r="K77" s="37"/>
-      <c r="L77" s="37"/>
-      <c r="M77" s="37"/>
-      <c r="N77" s="46"/>
-      <c r="O77" s="44"/>
-      <c r="P77" s="29"/>
-      <c r="Q77" s="37"/>
-      <c r="R77" s="77"/>
-      <c r="S77" s="78"/>
-      <c r="T77" s="44"/>
-      <c r="U77" s="89"/>
+      <c r="H77" s="43"/>
+      <c r="I77" s="91"/>
+      <c r="J77" s="92"/>
+      <c r="K77" s="29"/>
+      <c r="L77" s="29"/>
+      <c r="M77" s="29"/>
+      <c r="N77" s="43"/>
+      <c r="O77" s="43"/>
+      <c r="P77" s="39"/>
+      <c r="Q77" s="29"/>
+      <c r="R77" s="91"/>
+      <c r="S77" s="92"/>
+      <c r="T77" s="43"/>
+      <c r="U77" s="75"/>
       <c r="V77" s="76"/>
       <c r="W77" s="75"/>
       <c r="X77" s="76"/>
-      <c r="Y77" s="46"/>
+      <c r="Y77" s="43"/>
       <c r="Z77" s="29"/>
     </row>
     <row r="78" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="9"/>
+      <c r="B78" s="57"/>
+      <c r="C78" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G78" s="43"/>
       <c r="H78" s="43"/>
-      <c r="I78" s="77"/>
-      <c r="J78" s="78"/>
+      <c r="I78" s="91"/>
+      <c r="J78" s="92"/>
       <c r="K78" s="29"/>
       <c r="L78" s="29"/>
       <c r="M78" s="29"/>
       <c r="N78" s="43"/>
       <c r="O78" s="43"/>
-      <c r="P78" s="29"/>
+      <c r="P78" s="39"/>
       <c r="Q78" s="29"/>
-      <c r="R78" s="77"/>
-      <c r="S78" s="78"/>
+      <c r="R78" s="91"/>
+      <c r="S78" s="92"/>
       <c r="T78" s="43"/>
       <c r="U78" s="75"/>
       <c r="V78" s="76"/>
@@ -3731,11 +3728,9 @@
       <c r="Y78" s="43"/>
       <c r="Z78" s="29"/>
     </row>
-    <row r="79" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="9"/>
-      <c r="B79" s="60" t="s">
-        <v>56</v>
-      </c>
+      <c r="B79" s="57"/>
       <c r="C79" s="2" t="s">
         <v>50</v>
       </c>
@@ -3747,17 +3742,17 @@
       </c>
       <c r="G79" s="43"/>
       <c r="H79" s="43"/>
-      <c r="I79" s="77"/>
-      <c r="J79" s="78"/>
+      <c r="I79" s="91"/>
+      <c r="J79" s="92"/>
       <c r="K79" s="29"/>
       <c r="L79" s="29"/>
       <c r="M79" s="29"/>
       <c r="N79" s="43"/>
       <c r="O79" s="43"/>
       <c r="P79" s="39"/>
-      <c r="Q79" s="29"/>
-      <c r="R79" s="77"/>
-      <c r="S79" s="78"/>
+      <c r="Q79" s="39"/>
+      <c r="R79" s="91"/>
+      <c r="S79" s="92"/>
       <c r="T79" s="43"/>
       <c r="U79" s="75"/>
       <c r="V79" s="76"/>
@@ -3770,7 +3765,7 @@
       <c r="A80" s="9"/>
       <c r="B80" s="57"/>
       <c r="C80" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>23</v>
@@ -3780,17 +3775,17 @@
       </c>
       <c r="G80" s="43"/>
       <c r="H80" s="43"/>
-      <c r="I80" s="77"/>
-      <c r="J80" s="78"/>
+      <c r="I80" s="91"/>
+      <c r="J80" s="92"/>
       <c r="K80" s="29"/>
       <c r="L80" s="29"/>
       <c r="M80" s="29"/>
       <c r="N80" s="43"/>
       <c r="O80" s="43"/>
       <c r="P80" s="39"/>
-      <c r="Q80" s="29"/>
-      <c r="R80" s="77"/>
-      <c r="S80" s="78"/>
+      <c r="Q80" s="39"/>
+      <c r="R80" s="91"/>
+      <c r="S80" s="92"/>
       <c r="T80" s="43"/>
       <c r="U80" s="75"/>
       <c r="V80" s="76"/>
@@ -3803,18 +3798,18 @@
       <c r="A81" s="9"/>
       <c r="B81" s="57"/>
       <c r="C81" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="G81" s="43"/>
       <c r="H81" s="43"/>
-      <c r="I81" s="77"/>
-      <c r="J81" s="78"/>
+      <c r="I81" s="91"/>
+      <c r="J81" s="92"/>
       <c r="K81" s="29"/>
       <c r="L81" s="29"/>
       <c r="M81" s="29"/>
@@ -3822,8 +3817,8 @@
       <c r="O81" s="43"/>
       <c r="P81" s="39"/>
       <c r="Q81" s="39"/>
-      <c r="R81" s="77"/>
-      <c r="S81" s="78"/>
+      <c r="R81" s="91"/>
+      <c r="S81" s="92"/>
       <c r="T81" s="43"/>
       <c r="U81" s="75"/>
       <c r="V81" s="76"/>
@@ -3836,18 +3831,18 @@
       <c r="A82" s="9"/>
       <c r="B82" s="57"/>
       <c r="C82" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="G82" s="43"/>
       <c r="H82" s="43"/>
-      <c r="I82" s="77"/>
-      <c r="J82" s="78"/>
+      <c r="I82" s="91"/>
+      <c r="J82" s="92"/>
       <c r="K82" s="29"/>
       <c r="L82" s="29"/>
       <c r="M82" s="29"/>
@@ -3855,8 +3850,8 @@
       <c r="O82" s="43"/>
       <c r="P82" s="39"/>
       <c r="Q82" s="39"/>
-      <c r="R82" s="77"/>
-      <c r="S82" s="78"/>
+      <c r="R82" s="91"/>
+      <c r="S82" s="92"/>
       <c r="T82" s="43"/>
       <c r="U82" s="75"/>
       <c r="V82" s="76"/>
@@ -3867,29 +3862,19 @@
     </row>
     <row r="83" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="9"/>
-      <c r="B83" s="57"/>
-      <c r="C83" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="G83" s="43"/>
       <c r="H83" s="43"/>
-      <c r="I83" s="77"/>
-      <c r="J83" s="78"/>
+      <c r="I83" s="91"/>
+      <c r="J83" s="92"/>
       <c r="K83" s="29"/>
       <c r="L83" s="29"/>
       <c r="M83" s="29"/>
       <c r="N83" s="43"/>
       <c r="O83" s="43"/>
-      <c r="P83" s="39"/>
-      <c r="Q83" s="39"/>
-      <c r="R83" s="77"/>
-      <c r="S83" s="78"/>
+      <c r="P83" s="29"/>
+      <c r="Q83" s="29"/>
+      <c r="R83" s="91"/>
+      <c r="S83" s="92"/>
       <c r="T83" s="43"/>
       <c r="U83" s="75"/>
       <c r="V83" s="76"/>
@@ -3898,31 +3883,33 @@
       <c r="Y83" s="43"/>
       <c r="Z83" s="29"/>
     </row>
-    <row r="84" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A84" s="9"/>
-      <c r="B84" s="57"/>
+      <c r="B84" s="59" t="s">
+        <v>56</v>
+      </c>
       <c r="C84" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="G84" s="43"/>
       <c r="H84" s="43"/>
-      <c r="I84" s="77"/>
-      <c r="J84" s="78"/>
+      <c r="I84" s="91"/>
+      <c r="J84" s="92"/>
       <c r="K84" s="29"/>
       <c r="L84" s="29"/>
       <c r="M84" s="29"/>
       <c r="N84" s="43"/>
       <c r="O84" s="43"/>
       <c r="P84" s="39"/>
-      <c r="Q84" s="39"/>
-      <c r="R84" s="77"/>
-      <c r="S84" s="78"/>
+      <c r="Q84" s="29"/>
+      <c r="R84" s="91"/>
+      <c r="S84" s="92"/>
       <c r="T84" s="43"/>
       <c r="U84" s="75"/>
       <c r="V84" s="76"/>
@@ -3933,19 +3920,29 @@
     </row>
     <row r="85" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="9"/>
+      <c r="B85" s="58"/>
+      <c r="C85" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G85" s="43"/>
       <c r="H85" s="43"/>
-      <c r="I85" s="77"/>
-      <c r="J85" s="78"/>
+      <c r="I85" s="91"/>
+      <c r="J85" s="92"/>
       <c r="K85" s="29"/>
       <c r="L85" s="29"/>
       <c r="M85" s="29"/>
       <c r="N85" s="43"/>
       <c r="O85" s="43"/>
-      <c r="P85" s="29"/>
+      <c r="P85" s="39"/>
       <c r="Q85" s="29"/>
-      <c r="R85" s="77"/>
-      <c r="S85" s="78"/>
+      <c r="R85" s="91"/>
+      <c r="S85" s="92"/>
       <c r="T85" s="43"/>
       <c r="U85" s="75"/>
       <c r="V85" s="76"/>
@@ -3954,11 +3951,9 @@
       <c r="Y85" s="43"/>
       <c r="Z85" s="29"/>
     </row>
-    <row r="86" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="9"/>
-      <c r="B86" s="59" t="s">
-        <v>57</v>
-      </c>
+      <c r="B86" s="58"/>
       <c r="C86" s="2" t="s">
         <v>50</v>
       </c>
@@ -3970,17 +3965,17 @@
       </c>
       <c r="G86" s="43"/>
       <c r="H86" s="43"/>
-      <c r="I86" s="77"/>
-      <c r="J86" s="78"/>
+      <c r="I86" s="91"/>
+      <c r="J86" s="92"/>
       <c r="K86" s="29"/>
       <c r="L86" s="29"/>
       <c r="M86" s="29"/>
       <c r="N86" s="43"/>
       <c r="O86" s="43"/>
       <c r="P86" s="39"/>
-      <c r="Q86" s="29"/>
-      <c r="R86" s="77"/>
-      <c r="S86" s="78"/>
+      <c r="Q86" s="39"/>
+      <c r="R86" s="91"/>
+      <c r="S86" s="92"/>
       <c r="T86" s="43"/>
       <c r="U86" s="75"/>
       <c r="V86" s="76"/>
@@ -3993,7 +3988,7 @@
       <c r="A87" s="9"/>
       <c r="B87" s="58"/>
       <c r="C87" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>23</v>
@@ -4003,17 +3998,17 @@
       </c>
       <c r="G87" s="43"/>
       <c r="H87" s="43"/>
-      <c r="I87" s="77"/>
-      <c r="J87" s="78"/>
+      <c r="I87" s="91"/>
+      <c r="J87" s="92"/>
       <c r="K87" s="29"/>
       <c r="L87" s="29"/>
       <c r="M87" s="29"/>
       <c r="N87" s="43"/>
       <c r="O87" s="43"/>
       <c r="P87" s="39"/>
-      <c r="Q87" s="29"/>
-      <c r="R87" s="77"/>
-      <c r="S87" s="78"/>
+      <c r="Q87" s="39"/>
+      <c r="R87" s="91"/>
+      <c r="S87" s="92"/>
       <c r="T87" s="43"/>
       <c r="U87" s="75"/>
       <c r="V87" s="76"/>
@@ -4026,18 +4021,18 @@
       <c r="A88" s="9"/>
       <c r="B88" s="58"/>
       <c r="C88" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="G88" s="43"/>
       <c r="H88" s="43"/>
-      <c r="I88" s="77"/>
-      <c r="J88" s="78"/>
+      <c r="I88" s="91"/>
+      <c r="J88" s="92"/>
       <c r="K88" s="29"/>
       <c r="L88" s="29"/>
       <c r="M88" s="29"/>
@@ -4045,8 +4040,8 @@
       <c r="O88" s="43"/>
       <c r="P88" s="39"/>
       <c r="Q88" s="39"/>
-      <c r="R88" s="77"/>
-      <c r="S88" s="78"/>
+      <c r="R88" s="91"/>
+      <c r="S88" s="92"/>
       <c r="T88" s="43"/>
       <c r="U88" s="75"/>
       <c r="V88" s="76"/>
@@ -4059,18 +4054,18 @@
       <c r="A89" s="9"/>
       <c r="B89" s="58"/>
       <c r="C89" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="G89" s="43"/>
       <c r="H89" s="43"/>
-      <c r="I89" s="77"/>
-      <c r="J89" s="78"/>
+      <c r="I89" s="91"/>
+      <c r="J89" s="92"/>
       <c r="K89" s="29"/>
       <c r="L89" s="29"/>
       <c r="M89" s="29"/>
@@ -4078,8 +4073,8 @@
       <c r="O89" s="43"/>
       <c r="P89" s="39"/>
       <c r="Q89" s="39"/>
-      <c r="R89" s="77"/>
-      <c r="S89" s="78"/>
+      <c r="R89" s="91"/>
+      <c r="S89" s="92"/>
       <c r="T89" s="43"/>
       <c r="U89" s="75"/>
       <c r="V89" s="76"/>
@@ -4088,74 +4083,8 @@
       <c r="Y89" s="43"/>
       <c r="Z89" s="29"/>
     </row>
-    <row r="90" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" s="9"/>
-      <c r="B90" s="58"/>
-      <c r="C90" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G90" s="43"/>
-      <c r="H90" s="43"/>
-      <c r="I90" s="77"/>
-      <c r="J90" s="78"/>
-      <c r="K90" s="29"/>
-      <c r="L90" s="29"/>
-      <c r="M90" s="29"/>
-      <c r="N90" s="43"/>
-      <c r="O90" s="43"/>
-      <c r="P90" s="39"/>
-      <c r="Q90" s="39"/>
-      <c r="R90" s="77"/>
-      <c r="S90" s="78"/>
-      <c r="T90" s="43"/>
-      <c r="U90" s="75"/>
-      <c r="V90" s="76"/>
-      <c r="W90" s="75"/>
-      <c r="X90" s="76"/>
-      <c r="Y90" s="43"/>
-      <c r="Z90" s="29"/>
-    </row>
-    <row r="91" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A91" s="9"/>
-      <c r="B91" s="58"/>
-      <c r="C91" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G91" s="43"/>
-      <c r="H91" s="43"/>
-      <c r="I91" s="77"/>
-      <c r="J91" s="78"/>
-      <c r="K91" s="29"/>
-      <c r="L91" s="29"/>
-      <c r="M91" s="29"/>
-      <c r="N91" s="43"/>
-      <c r="O91" s="43"/>
-      <c r="P91" s="39"/>
-      <c r="Q91" s="39"/>
-      <c r="R91" s="77"/>
-      <c r="S91" s="78"/>
-      <c r="T91" s="43"/>
-      <c r="U91" s="75"/>
-      <c r="V91" s="76"/>
-      <c r="W91" s="75"/>
-      <c r="X91" s="76"/>
-      <c r="Y91" s="43"/>
-      <c r="Z91" s="29"/>
-    </row>
   </sheetData>
-  <mergeCells count="341">
+  <mergeCells count="333">
     <mergeCell ref="G5:K5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="N5:O5"/>
@@ -4165,6 +4094,10 @@
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="W3:X3"/>
     <mergeCell ref="W4:X4"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="I6:J6"/>
@@ -4177,78 +4110,72 @@
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="I15:J15"/>
     <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I40:J40"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="I23:J23"/>
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="I25:J25"/>
     <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
     <mergeCell ref="I41:J41"/>
     <mergeCell ref="I42:J42"/>
     <mergeCell ref="I43:J43"/>
-    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="I36:J36"/>
     <mergeCell ref="I37:J37"/>
     <mergeCell ref="I38:J38"/>
     <mergeCell ref="I39:J39"/>
-    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="I51:J51"/>
     <mergeCell ref="I52:J52"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="I60:J60"/>
     <mergeCell ref="I53:J53"/>
     <mergeCell ref="I54:J54"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="I56:J56"/>
     <mergeCell ref="I61:J61"/>
     <mergeCell ref="I62:J62"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="I56:J56"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="I69:J69"/>
     <mergeCell ref="I63:J63"/>
     <mergeCell ref="I64:J64"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="I72:J72"/>
     <mergeCell ref="I70:J70"/>
     <mergeCell ref="I71:J71"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="I67:J67"/>
     <mergeCell ref="I74:J74"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="I75:J75"/>
     <mergeCell ref="I76:J76"/>
     <mergeCell ref="I77:J77"/>
     <mergeCell ref="I78:J78"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="I89:J89"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I85:J85"/>
+    <mergeCell ref="I86:J86"/>
+    <mergeCell ref="I87:J87"/>
+    <mergeCell ref="I88:J88"/>
+    <mergeCell ref="I84:J84"/>
     <mergeCell ref="I79:J79"/>
     <mergeCell ref="I80:J80"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="I91:J91"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I87:J87"/>
-    <mergeCell ref="I88:J88"/>
-    <mergeCell ref="I89:J89"/>
-    <mergeCell ref="I90:J90"/>
-    <mergeCell ref="I86:J86"/>
     <mergeCell ref="I81:J81"/>
     <mergeCell ref="I82:J82"/>
     <mergeCell ref="I83:J83"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="I85:J85"/>
     <mergeCell ref="R11:S11"/>
     <mergeCell ref="R13:S13"/>
     <mergeCell ref="R12:S12"/>
@@ -4269,69 +4196,67 @@
     <mergeCell ref="R19:S19"/>
     <mergeCell ref="R20:S20"/>
     <mergeCell ref="R21:S21"/>
+    <mergeCell ref="R35:S35"/>
+    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="R46:S46"/>
     <mergeCell ref="R32:S32"/>
     <mergeCell ref="R33:S33"/>
     <mergeCell ref="R34:S34"/>
-    <mergeCell ref="R35:S35"/>
     <mergeCell ref="R27:S27"/>
     <mergeCell ref="R28:S28"/>
     <mergeCell ref="R29:S29"/>
     <mergeCell ref="R30:S30"/>
     <mergeCell ref="R31:S31"/>
+    <mergeCell ref="R47:S47"/>
+    <mergeCell ref="R48:S48"/>
+    <mergeCell ref="R49:S49"/>
+    <mergeCell ref="R43:S43"/>
+    <mergeCell ref="R44:S44"/>
+    <mergeCell ref="R45:S45"/>
+    <mergeCell ref="R54:S54"/>
+    <mergeCell ref="R55:S55"/>
+    <mergeCell ref="R38:S38"/>
     <mergeCell ref="R39:S39"/>
     <mergeCell ref="R40:S40"/>
     <mergeCell ref="R41:S41"/>
     <mergeCell ref="R42:S42"/>
-    <mergeCell ref="R43:S43"/>
-    <mergeCell ref="R36:S36"/>
-    <mergeCell ref="R37:S37"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="R48:S48"/>
-    <mergeCell ref="R49:S49"/>
+    <mergeCell ref="R57:S57"/>
+    <mergeCell ref="R58:S58"/>
     <mergeCell ref="R50:S50"/>
     <mergeCell ref="R51:S51"/>
-    <mergeCell ref="R44:S44"/>
-    <mergeCell ref="R45:S45"/>
-    <mergeCell ref="R46:S46"/>
-    <mergeCell ref="R47:S47"/>
-    <mergeCell ref="R56:S56"/>
-    <mergeCell ref="R57:S57"/>
+    <mergeCell ref="R52:S52"/>
+    <mergeCell ref="R53:S53"/>
     <mergeCell ref="R59:S59"/>
     <mergeCell ref="R60:S60"/>
-    <mergeCell ref="R52:S52"/>
-    <mergeCell ref="R53:S53"/>
-    <mergeCell ref="R54:S54"/>
-    <mergeCell ref="R55:S55"/>
+    <mergeCell ref="R64:S64"/>
+    <mergeCell ref="R65:S65"/>
+    <mergeCell ref="R66:S66"/>
+    <mergeCell ref="R67:S67"/>
     <mergeCell ref="R61:S61"/>
     <mergeCell ref="R62:S62"/>
-    <mergeCell ref="R66:S66"/>
-    <mergeCell ref="R67:S67"/>
     <mergeCell ref="R68:S68"/>
     <mergeCell ref="R69:S69"/>
-    <mergeCell ref="R63:S63"/>
-    <mergeCell ref="R64:S64"/>
     <mergeCell ref="R70:S70"/>
     <mergeCell ref="R71:S71"/>
+    <mergeCell ref="R73:S73"/>
+    <mergeCell ref="R74:S74"/>
+    <mergeCell ref="R75:S75"/>
     <mergeCell ref="R72:S72"/>
-    <mergeCell ref="R73:S73"/>
-    <mergeCell ref="R75:S75"/>
+    <mergeCell ref="R81:S81"/>
+    <mergeCell ref="R82:S82"/>
+    <mergeCell ref="R83:S83"/>
     <mergeCell ref="R76:S76"/>
     <mergeCell ref="R77:S77"/>
-    <mergeCell ref="R74:S74"/>
-    <mergeCell ref="R83:S83"/>
-    <mergeCell ref="R84:S84"/>
-    <mergeCell ref="R85:S85"/>
     <mergeCell ref="R78:S78"/>
     <mergeCell ref="R79:S79"/>
     <mergeCell ref="R80:S80"/>
-    <mergeCell ref="R81:S81"/>
-    <mergeCell ref="R82:S82"/>
+    <mergeCell ref="R86:S86"/>
+    <mergeCell ref="R87:S87"/>
     <mergeCell ref="R88:S88"/>
     <mergeCell ref="R89:S89"/>
-    <mergeCell ref="R90:S90"/>
-    <mergeCell ref="R91:S91"/>
-    <mergeCell ref="R86:S86"/>
-    <mergeCell ref="R87:S87"/>
+    <mergeCell ref="R84:S84"/>
+    <mergeCell ref="R85:S85"/>
     <mergeCell ref="U7:V7"/>
     <mergeCell ref="U8:V8"/>
     <mergeCell ref="U6:V6"/>
@@ -4350,76 +4275,74 @@
     <mergeCell ref="U25:V25"/>
     <mergeCell ref="U26:V26"/>
     <mergeCell ref="U18:V18"/>
+    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="U37:V37"/>
+    <mergeCell ref="U38:V38"/>
+    <mergeCell ref="U39:V39"/>
+    <mergeCell ref="U50:V50"/>
     <mergeCell ref="U19:V19"/>
     <mergeCell ref="U20:V20"/>
     <mergeCell ref="U21:V21"/>
     <mergeCell ref="U32:V32"/>
-    <mergeCell ref="U33:V33"/>
-    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="U35:V35"/>
     <mergeCell ref="U27:V27"/>
     <mergeCell ref="U28:V28"/>
     <mergeCell ref="U29:V29"/>
     <mergeCell ref="U30:V30"/>
     <mergeCell ref="U31:V31"/>
+    <mergeCell ref="U51:V51"/>
+    <mergeCell ref="U52:V52"/>
+    <mergeCell ref="U44:V44"/>
+    <mergeCell ref="U45:V45"/>
+    <mergeCell ref="U48:V48"/>
+    <mergeCell ref="U49:V49"/>
+    <mergeCell ref="U57:V57"/>
+    <mergeCell ref="U59:V59"/>
+    <mergeCell ref="U40:V40"/>
     <mergeCell ref="U41:V41"/>
     <mergeCell ref="U42:V42"/>
     <mergeCell ref="U43:V43"/>
-    <mergeCell ref="U44:V44"/>
-    <mergeCell ref="U37:V37"/>
-    <mergeCell ref="U38:V38"/>
-    <mergeCell ref="U39:V39"/>
-    <mergeCell ref="U40:V40"/>
-    <mergeCell ref="U52:V52"/>
+    <mergeCell ref="U60:V60"/>
     <mergeCell ref="U53:V53"/>
     <mergeCell ref="U54:V54"/>
-    <mergeCell ref="U45:V45"/>
-    <mergeCell ref="U46:V46"/>
-    <mergeCell ref="U47:V47"/>
-    <mergeCell ref="U50:V50"/>
-    <mergeCell ref="U51:V51"/>
-    <mergeCell ref="U59:V59"/>
+    <mergeCell ref="U55:V55"/>
+    <mergeCell ref="U56:V56"/>
     <mergeCell ref="U61:V61"/>
     <mergeCell ref="U62:V62"/>
-    <mergeCell ref="U55:V55"/>
-    <mergeCell ref="U56:V56"/>
-    <mergeCell ref="U57:V57"/>
-    <mergeCell ref="U58:V58"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="U68:V68"/>
+    <mergeCell ref="U69:V69"/>
     <mergeCell ref="U63:V63"/>
     <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U68:V68"/>
-    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="U65:V65"/>
+    <mergeCell ref="U72:V72"/>
     <mergeCell ref="U70:V70"/>
     <mergeCell ref="U71:V71"/>
-    <mergeCell ref="U65:V65"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="U67:V67"/>
     <mergeCell ref="U74:V74"/>
-    <mergeCell ref="U72:V72"/>
-    <mergeCell ref="U73:V73"/>
+    <mergeCell ref="U75:V75"/>
     <mergeCell ref="U76:V76"/>
     <mergeCell ref="U77:V77"/>
     <mergeCell ref="U78:V78"/>
+    <mergeCell ref="U73:V73"/>
+    <mergeCell ref="U87:V87"/>
+    <mergeCell ref="U88:V88"/>
+    <mergeCell ref="U84:V84"/>
     <mergeCell ref="U79:V79"/>
     <mergeCell ref="U80:V80"/>
-    <mergeCell ref="U75:V75"/>
-    <mergeCell ref="U89:V89"/>
-    <mergeCell ref="U90:V90"/>
-    <mergeCell ref="U86:V86"/>
     <mergeCell ref="U81:V81"/>
     <mergeCell ref="U82:V82"/>
     <mergeCell ref="U83:V83"/>
-    <mergeCell ref="U84:V84"/>
-    <mergeCell ref="U85:V85"/>
     <mergeCell ref="W12:X12"/>
-    <mergeCell ref="U91:V91"/>
+    <mergeCell ref="U89:V89"/>
     <mergeCell ref="W6:X6"/>
     <mergeCell ref="W7:X7"/>
     <mergeCell ref="W8:X8"/>
     <mergeCell ref="W9:X9"/>
     <mergeCell ref="W10:X10"/>
     <mergeCell ref="W11:X11"/>
-    <mergeCell ref="U87:V87"/>
-    <mergeCell ref="U88:V88"/>
+    <mergeCell ref="U85:V85"/>
+    <mergeCell ref="U86:V86"/>
     <mergeCell ref="W16:X16"/>
     <mergeCell ref="W17:X17"/>
     <mergeCell ref="W13:X13"/>
@@ -4434,69 +4357,67 @@
     <mergeCell ref="W19:X19"/>
     <mergeCell ref="W20:X20"/>
     <mergeCell ref="W31:X31"/>
+    <mergeCell ref="W34:X34"/>
+    <mergeCell ref="W35:X35"/>
+    <mergeCell ref="W36:X36"/>
+    <mergeCell ref="W45:X45"/>
+    <mergeCell ref="W46:X46"/>
     <mergeCell ref="W32:X32"/>
     <mergeCell ref="W33:X33"/>
-    <mergeCell ref="W34:X34"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="W27:X27"/>
     <mergeCell ref="W28:X28"/>
     <mergeCell ref="W29:X29"/>
     <mergeCell ref="W30:X30"/>
+    <mergeCell ref="W37:X37"/>
+    <mergeCell ref="W47:X47"/>
+    <mergeCell ref="W48:X48"/>
+    <mergeCell ref="W49:X49"/>
+    <mergeCell ref="W42:X42"/>
+    <mergeCell ref="W43:X43"/>
+    <mergeCell ref="W44:X44"/>
+    <mergeCell ref="W53:X53"/>
+    <mergeCell ref="W54:X54"/>
     <mergeCell ref="W38:X38"/>
     <mergeCell ref="W39:X39"/>
     <mergeCell ref="W40:X40"/>
     <mergeCell ref="W41:X41"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="W35:X35"/>
-    <mergeCell ref="W36:X36"/>
-    <mergeCell ref="W37:X37"/>
-    <mergeCell ref="W47:X47"/>
-    <mergeCell ref="W48:X48"/>
-    <mergeCell ref="W49:X49"/>
+    <mergeCell ref="W55:X55"/>
+    <mergeCell ref="W57:X57"/>
     <mergeCell ref="W50:X50"/>
     <mergeCell ref="W51:X51"/>
-    <mergeCell ref="W43:X43"/>
-    <mergeCell ref="W44:X44"/>
-    <mergeCell ref="W45:X45"/>
-    <mergeCell ref="W46:X46"/>
-    <mergeCell ref="W55:X55"/>
-    <mergeCell ref="W56:X56"/>
-    <mergeCell ref="W57:X57"/>
+    <mergeCell ref="W52:X52"/>
+    <mergeCell ref="W58:X58"/>
     <mergeCell ref="W59:X59"/>
-    <mergeCell ref="W52:X52"/>
-    <mergeCell ref="W53:X53"/>
-    <mergeCell ref="W54:X54"/>
     <mergeCell ref="W60:X60"/>
+    <mergeCell ref="W64:X64"/>
+    <mergeCell ref="W65:X65"/>
+    <mergeCell ref="W66:X66"/>
     <mergeCell ref="W61:X61"/>
     <mergeCell ref="W62:X62"/>
-    <mergeCell ref="W66:X66"/>
+    <mergeCell ref="W71:X71"/>
     <mergeCell ref="W67:X67"/>
     <mergeCell ref="W68:X68"/>
-    <mergeCell ref="W63:X63"/>
-    <mergeCell ref="W64:X64"/>
-    <mergeCell ref="W73:X73"/>
     <mergeCell ref="W69:X69"/>
     <mergeCell ref="W70:X70"/>
-    <mergeCell ref="W71:X71"/>
+    <mergeCell ref="W73:X73"/>
+    <mergeCell ref="W74:X74"/>
     <mergeCell ref="W72:X72"/>
+    <mergeCell ref="W86:X86"/>
+    <mergeCell ref="W87:X87"/>
+    <mergeCell ref="W88:X88"/>
+    <mergeCell ref="W89:X89"/>
+    <mergeCell ref="W84:X84"/>
+    <mergeCell ref="W85:X85"/>
+    <mergeCell ref="W80:X80"/>
+    <mergeCell ref="W81:X81"/>
+    <mergeCell ref="W82:X82"/>
+    <mergeCell ref="W83:X83"/>
     <mergeCell ref="W75:X75"/>
     <mergeCell ref="W76:X76"/>
-    <mergeCell ref="W74:X74"/>
-    <mergeCell ref="W88:X88"/>
-    <mergeCell ref="W89:X89"/>
-    <mergeCell ref="W90:X90"/>
-    <mergeCell ref="W91:X91"/>
-    <mergeCell ref="W86:X86"/>
-    <mergeCell ref="W87:X87"/>
-    <mergeCell ref="W82:X82"/>
-    <mergeCell ref="W83:X83"/>
-    <mergeCell ref="W84:X84"/>
-    <mergeCell ref="W85:X85"/>
     <mergeCell ref="W77:X77"/>
     <mergeCell ref="W78:X78"/>
     <mergeCell ref="W79:X79"/>
-    <mergeCell ref="W80:X80"/>
-    <mergeCell ref="W81:X81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>